<commit_message>
update sprint report 2
</commit_message>
<xml_diff>
--- a/src/doc/Sprint2.xlsx
+++ b/src/doc/Sprint2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POE\git\Comp-3004A-Team-40-Rummy\src\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Fall18\comp3004\Comp-3004A-Team-40-Rummy\src\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$34</definedName>
   </definedNames>
   <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
@@ -27,47 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
   <si>
     <t xml:space="preserve">item </t>
   </si>
   <si>
-    <t>Create Repository</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>Add team members as Contributors</t>
-  </si>
-  <si>
-    <t>Frist Strategy test cases</t>
-  </si>
-  <si>
-    <t>Second Strategy test cases</t>
-  </si>
-  <si>
-    <t>Third Stategy Test cases</t>
-  </si>
-  <si>
-    <t>Player strategy test cases</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Deck class test cases</t>
-  </si>
-  <si>
-    <t>Tile class test cases</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -80,40 +53,109 @@
     <t>Dallaire Jacob</t>
   </si>
   <si>
-    <t>Dairo Emmanue</t>
-  </si>
-  <si>
     <t>TA</t>
   </si>
   <si>
     <t>Mitchell</t>
   </si>
   <si>
-    <t>Player test cases updated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 meetings </t>
-  </si>
-  <si>
-    <t>Create Game class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Strategy </t>
-  </si>
-  <si>
-    <t>Table test cases updated</t>
-  </si>
-  <si>
-    <t>Create test cases for game logic</t>
-  </si>
-  <si>
-    <t>Create test cases for player moves</t>
-  </si>
-  <si>
     <t>Oct 9 - Oct 18</t>
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Merged run with loop to cycle through the players properly</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Added Run and play functions to the game class</t>
+  </si>
+  <si>
+    <t>Modified the Play function.</t>
+  </si>
+  <si>
+    <t>testing game loop: fail</t>
+  </si>
+  <si>
+    <t>testing game loop: pass</t>
+  </si>
+  <si>
+    <t>update sprint report, fix errors in TestTable.java</t>
+  </si>
+  <si>
+    <t>refactoring Table, Strategy extends Strategy, comments</t>
+  </si>
+  <si>
+    <t>strategy: is now an abstract class</t>
+  </si>
+  <si>
+    <t>color and value comparator:for sorting hand</t>
+  </si>
+  <si>
+    <t>firststrategy:refactored the code</t>
+  </si>
+  <si>
+    <t>Added test for player first30 flag</t>
+  </si>
+  <si>
+    <t>Added flag to player to determine if first 30 pts played</t>
+  </si>
+  <si>
+    <t>Re did data structure for melds as well as adding a new meld</t>
+  </si>
+  <si>
+    <t>Refactoring of stategy classes</t>
+  </si>
+  <si>
+    <t>Added tests for game input and player input.</t>
+  </si>
+  <si>
+    <t>Created a game class that will handle the player playing the game against the ai</t>
+  </si>
+  <si>
+    <t>eclipse javafx jar file</t>
+  </si>
+  <si>
+    <t>add shapes as collections and display on canvas</t>
+  </si>
+  <si>
+    <t>Resolved differences in master file</t>
+  </si>
+  <si>
+    <t>app: started game fuctionality</t>
+  </si>
+  <si>
+    <t>deck: created helper functions</t>
+  </si>
+  <si>
+    <t>table: created helper functions</t>
+  </si>
+  <si>
+    <t>Dairo Emmanuel</t>
+  </si>
+  <si>
+    <t>bug fix in table test</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>Integrate code to create single playable class</t>
+  </si>
+  <si>
+    <t>ISSUES:</t>
+  </si>
+  <si>
+    <t>Lots of code not preceded by relevant tests</t>
+  </si>
+  <si>
+    <t>Strategy class implementation not clear to group members - some clonflicts with Player class</t>
+  </si>
+  <si>
+    <t>Tough week with all those midterms!</t>
   </si>
 </sst>
 </file>
@@ -157,12 +199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,16 +229,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>254001</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>365125</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>87155</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>103030</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -210,7 +255,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7159626" y="0"/>
+          <a:off x="12303126" y="1920875"/>
           <a:ext cx="10969624" cy="6373655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -486,218 +531,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>